<commit_message>
Update the schedule with the current status for the project
</commit_message>
<xml_diff>
--- a/Project Plan/Project Schedule.xlsx
+++ b/Project Plan/Project Schedule.xlsx
@@ -328,7 +328,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="68">
   <si>
     <t>NA</t>
   </si>
@@ -437,9 +437,6 @@
   </si>
   <si>
     <t>CRS-SIQ</t>
-  </si>
-  <si>
-    <t>Postponed</t>
   </si>
   <si>
     <t>Yasser &amp; Mariam</t>
@@ -1049,6 +1046,33 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1056,33 +1080,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1396,8 +1393,8 @@
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q36" sqref="Q36"/>
+      <pane ySplit="8" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -1449,34 +1446,34 @@
       <c r="B3" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="56"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="53"/>
     </row>
     <row r="4" spans="1:18" ht="12.75">
       <c r="B4" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="52"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="50"/>
     </row>
     <row r="5" spans="1:18" ht="12.75">
       <c r="B5" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="52"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -1485,13 +1482,13 @@
       <c r="B6" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="57">
+      <c r="C6" s="54">
         <f ca="1">NOW()</f>
-        <v>42461.626013425928</v>
-      </c>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="59"/>
+        <v>42462.01800625</v>
+      </c>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="56"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -1504,10 +1501,10 @@
       <c r="B8" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="49"/>
+      <c r="D8" s="58"/>
       <c r="E8" s="40" t="s">
         <v>23</v>
       </c>
@@ -1523,18 +1520,18 @@
       <c r="I8" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="49" t="s">
+      <c r="J8" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="49"/>
-      <c r="L8" s="48" t="s">
+      <c r="K8" s="58"/>
+      <c r="L8" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="48"/>
-      <c r="N8" s="48" t="s">
+      <c r="M8" s="57"/>
+      <c r="N8" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="48"/>
+      <c r="O8" s="57"/>
       <c r="P8" s="42" t="s">
         <v>15</v>
       </c>
@@ -1550,7 +1547,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="17">
         <v>35</v>
@@ -1594,7 +1591,7 @@
       </c>
       <c r="P9" s="18">
         <f>SUM(P12,P18,P24,P32)/4</f>
-        <v>0.58750000000000002</v>
+        <v>0.69374999999999998</v>
       </c>
       <c r="Q9" s="19"/>
       <c r="R9" s="15" t="s">
@@ -1606,7 +1603,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="17">
         <v>28</v>
@@ -1653,7 +1650,7 @@
       </c>
       <c r="Q10" s="19"/>
       <c r="R10" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:18" s="8" customFormat="1" ht="15.75">
@@ -1681,7 +1678,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="17">
         <v>7</v>
@@ -1736,7 +1733,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="17">
         <v>7</v>
@@ -1791,7 +1788,7 @@
         <v>1.2</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="17">
         <v>7</v>
@@ -1846,7 +1843,7 @@
         <v>1.3</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="17">
         <v>2</v>
@@ -1901,7 +1898,7 @@
         <v>1.4</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="17">
         <v>2</v>
@@ -1979,7 +1976,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="17">
         <v>7</v>
@@ -2010,21 +2007,21 @@
       </c>
       <c r="L18" s="17">
         <f>SUM(L19:L22)</f>
-        <v>15.5</v>
+        <v>16</v>
       </c>
       <c r="M18" s="17" t="s">
         <v>18</v>
       </c>
       <c r="N18" s="17">
         <f t="shared" si="0"/>
-        <v>-3.5</v>
+        <v>-4</v>
       </c>
       <c r="O18" s="17" t="s">
         <v>18</v>
       </c>
       <c r="P18" s="18">
         <f>AVERAGE(P19:P22)</f>
-        <v>0.89999999999999991</v>
+        <v>0.92499999999999993</v>
       </c>
       <c r="Q18" s="19">
         <v>1</v>
@@ -2083,7 +2080,7 @@
       </c>
       <c r="Q19" s="19"/>
       <c r="R19" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="15">
@@ -2091,7 +2088,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="17">
         <v>2</v>
@@ -2140,7 +2137,7 @@
         <v>2.1</v>
       </c>
       <c r="R20" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="15">
@@ -2148,7 +2145,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="17">
         <v>2</v>
@@ -2195,10 +2192,10 @@
         <v>0.9</v>
       </c>
       <c r="Q21" s="35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R21" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="15">
@@ -2237,26 +2234,26 @@
         <v>18</v>
       </c>
       <c r="L22" s="17">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="M22" s="17" t="s">
         <v>18</v>
       </c>
       <c r="N22" s="17">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O22" s="17" t="s">
         <v>18</v>
       </c>
       <c r="P22" s="18">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="Q22" s="19">
         <v>2.2000000000000002</v>
       </c>
       <c r="R22" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:18" s="8" customFormat="1" ht="15">
@@ -2284,7 +2281,7 @@
         <v>3</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="17">
         <v>14</v>
@@ -2315,21 +2312,21 @@
       </c>
       <c r="L24" s="17">
         <f>SUM(L25:L30)</f>
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="M24" s="17" t="s">
         <v>18</v>
       </c>
       <c r="N24" s="17">
         <f t="shared" ref="N24:N36" si="1">J24-L24</f>
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="O24" s="17" t="s">
         <v>18</v>
       </c>
       <c r="P24" s="23">
         <f>AVERAGE(P25:P30)</f>
-        <v>0.45</v>
+        <v>0.85000000000000009</v>
       </c>
       <c r="Q24" s="19">
         <v>2</v>
@@ -2341,7 +2338,7 @@
         <v>3.1</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="17">
         <v>4</v>
@@ -2396,7 +2393,7 @@
         <v>3.2</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="17">
         <v>4</v>
@@ -2418,8 +2415,8 @@
       <c r="H26" s="37">
         <v>42456</v>
       </c>
-      <c r="I26" s="37" t="s">
-        <v>0</v>
+      <c r="I26" s="37">
+        <v>42462</v>
       </c>
       <c r="J26" s="17">
         <v>6</v>
@@ -2428,26 +2425,26 @@
         <v>18</v>
       </c>
       <c r="L26" s="17">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M26" s="17" t="s">
         <v>18</v>
       </c>
       <c r="N26" s="17">
         <f t="shared" ref="N26:N30" si="2">J26-L26</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O26" s="17" t="s">
         <v>18</v>
       </c>
       <c r="P26" s="18">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="Q26" s="19">
         <v>3.1</v>
       </c>
       <c r="R26" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="15">
@@ -2455,7 +2452,7 @@
         <v>3.3</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C27" s="17">
         <v>1</v>
@@ -2463,21 +2460,21 @@
       <c r="D27" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="36" t="s">
-        <v>34</v>
+      <c r="E27" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="F27" s="37">
         <v>42456</v>
       </c>
-      <c r="G27" s="37" t="str">
+      <c r="G27" s="37">
         <f>I26</f>
-        <v>NA</v>
+        <v>42462</v>
       </c>
       <c r="H27" s="37">
         <v>42456</v>
       </c>
-      <c r="I27" s="37" t="s">
-        <v>0</v>
+      <c r="I27" s="37">
+        <v>42461</v>
       </c>
       <c r="J27" s="17">
         <v>2</v>
@@ -2486,26 +2483,26 @@
         <v>18</v>
       </c>
       <c r="L27" s="17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M27" s="17" t="s">
         <v>18</v>
       </c>
       <c r="N27" s="17">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O27" s="17" t="s">
         <v>18</v>
       </c>
       <c r="P27" s="18">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="Q27" s="19">
         <v>3.2</v>
       </c>
       <c r="R27" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="15">
@@ -2521,8 +2518,8 @@
       <c r="D28" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="36" t="s">
-        <v>34</v>
+      <c r="E28" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="F28" s="37">
         <v>42456</v>
@@ -2534,8 +2531,8 @@
       <c r="H28" s="37">
         <v>42458</v>
       </c>
-      <c r="I28" s="37" t="s">
-        <v>0</v>
+      <c r="I28" s="37">
+        <v>42461</v>
       </c>
       <c r="J28" s="17">
         <v>6</v>
@@ -2544,26 +2541,26 @@
         <v>18</v>
       </c>
       <c r="L28" s="17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M28" s="17" t="s">
         <v>18</v>
       </c>
       <c r="N28" s="17">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O28" s="17" t="s">
         <v>18</v>
       </c>
       <c r="P28" s="18">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="Q28" s="19">
         <v>3.2</v>
       </c>
       <c r="R28" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="15">
@@ -2571,7 +2568,7 @@
         <v>3.5</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="17">
         <v>1</v>
@@ -2579,14 +2576,15 @@
       <c r="D29" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="36" t="s">
-        <v>34</v>
+      <c r="E29" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="F29" s="37">
         <v>42458</v>
       </c>
-      <c r="G29" s="37" t="s">
-        <v>0</v>
+      <c r="G29" s="37">
+        <f>I28</f>
+        <v>42461</v>
       </c>
       <c r="H29" s="37">
         <v>42458</v>
@@ -2601,26 +2599,26 @@
         <v>18</v>
       </c>
       <c r="L29" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M29" s="17" t="s">
         <v>18</v>
       </c>
       <c r="N29" s="17">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O29" s="17" t="s">
         <v>18</v>
       </c>
       <c r="P29" s="18">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="Q29" s="19">
         <v>3.4</v>
       </c>
       <c r="R29" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="15">
@@ -2628,7 +2626,7 @@
         <v>3.6</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" s="17">
         <v>2</v>
@@ -2637,7 +2635,7 @@
         <v>8</v>
       </c>
       <c r="E30" s="36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F30" s="37">
         <v>42455</v>
@@ -2675,7 +2673,7 @@
       </c>
       <c r="Q30" s="19"/>
       <c r="R30" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:18" s="34" customFormat="1" ht="15">
@@ -2703,7 +2701,7 @@
         <v>2</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C32" s="17">
         <v>7</v>
@@ -2712,7 +2710,7 @@
         <v>8</v>
       </c>
       <c r="E32" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F32" s="37">
         <v>42462</v>
@@ -2757,7 +2755,7 @@
         <v>2.1</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" s="17">
         <v>1</v>
@@ -2766,7 +2764,7 @@
         <v>8</v>
       </c>
       <c r="E33" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F33" s="37">
         <v>42462</v>
@@ -2804,7 +2802,7 @@
       </c>
       <c r="Q33" s="19"/>
       <c r="R33" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="15">
@@ -2812,7 +2810,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C34" s="17">
         <v>2</v>
@@ -2821,7 +2819,7 @@
         <v>8</v>
       </c>
       <c r="E34" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F34" s="37">
         <v>42462</v>
@@ -2859,7 +2857,7 @@
       </c>
       <c r="Q34" s="35"/>
       <c r="R34" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="15">
@@ -2867,7 +2865,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C35" s="17">
         <v>2</v>
@@ -2876,7 +2874,7 @@
         <v>8</v>
       </c>
       <c r="E35" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F35" s="37">
         <v>42462</v>
@@ -2914,7 +2912,7 @@
       </c>
       <c r="Q35" s="19"/>
       <c r="R35" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="15">
@@ -2922,7 +2920,7 @@
         <v>2.4</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C36" s="17">
         <v>2</v>
@@ -2931,7 +2929,7 @@
         <v>8</v>
       </c>
       <c r="E36" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F36" s="37">
         <v>42462</v>
@@ -2969,7 +2967,7 @@
       </c>
       <c r="Q36" s="19"/>
       <c r="R36" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="15">

</xml_diff>

<commit_message>
Update the schedule with the progress in Stage 4
</commit_message>
<xml_diff>
--- a/Project Plan/Project Schedule.xlsx
+++ b/Project Plan/Project Schedule.xlsx
@@ -240,29 +240,6 @@
             <color indexed="81"/>
             <rFont val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Remaining Work
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The amount of time still required to complete a task.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
           <t xml:space="preserve">% Complete
 </t>
         </r>
@@ -277,7 +254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q8" authorId="0" shapeId="0">
+    <comment ref="O8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -300,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R8" authorId="0" shapeId="0">
+    <comment ref="P8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -328,7 +305,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="73">
   <si>
     <t>NA</t>
   </si>
@@ -377,10 +354,6 @@
 Work</t>
   </si>
   <si>
-    <t>Remaining
-Work</t>
-  </si>
-  <si>
     <t>%
 Complete</t>
   </si>
@@ -499,24 +472,15 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>Function Test</t>
-  </si>
-  <si>
     <t>Integration Test</t>
   </si>
   <si>
-    <t>Unit test</t>
-  </si>
-  <si>
     <t>User Acceptance Test</t>
   </si>
   <si>
     <t>All Team</t>
   </si>
   <si>
-    <t>Not yet</t>
-  </si>
-  <si>
     <t>Kareem</t>
   </si>
   <si>
@@ -539,6 +503,33 @@
   </si>
   <si>
     <t>Tareek &amp; Yasser</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>Update SRS</t>
+  </si>
+  <si>
+    <t>Update RTM</t>
+  </si>
+  <si>
+    <t>Update HLD</t>
+  </si>
+  <si>
+    <t>Update CDDs</t>
+  </si>
+  <si>
+    <t>Update Test cases</t>
+  </si>
+  <si>
+    <t>Hoda</t>
+  </si>
+  <si>
+    <t>Function test</t>
+  </si>
+  <si>
+    <t>Component test</t>
   </si>
 </sst>
 </file>
@@ -1390,11 +1381,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
+      <pane ySplit="8" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -1403,23 +1394,21 @@
     <col min="2" max="2" width="35.140625" style="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.140625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="5"/>
+    <col min="14" max="14" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" thickBot="1">
+    <row r="1" spans="1:16" ht="18.75" thickBot="1">
       <c r="A1" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="10"/>
@@ -1434,42 +1423,40 @@
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
       <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="13"/>
-    </row>
-    <row r="2" spans="1:18" ht="12" thickBot="1">
-      <c r="R2" s="4"/>
-    </row>
-    <row r="3" spans="1:18" ht="12.75">
+      <c r="O1" s="12"/>
+      <c r="P1" s="13"/>
+    </row>
+    <row r="2" spans="1:16" ht="12" thickBot="1">
+      <c r="P2" s="4"/>
+    </row>
+    <row r="3" spans="1:16" ht="12.75">
       <c r="B3" s="45" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="52"/>
       <c r="E3" s="52"/>
       <c r="F3" s="53"/>
     </row>
-    <row r="4" spans="1:18" ht="12.75">
+    <row r="4" spans="1:16" ht="12.75">
       <c r="B4" s="46" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="49"/>
       <c r="E4" s="49"/>
       <c r="F4" s="50"/>
     </row>
-    <row r="5" spans="1:18" ht="12.75">
+    <row r="5" spans="1:16" ht="12.75">
       <c r="B5" s="46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="49"/>
       <c r="E5" s="49"/>
@@ -1478,13 +1465,13 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:18" ht="13.5" thickBot="1">
+    <row r="6" spans="1:16" ht="13.5" thickBot="1">
       <c r="B6" s="47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="54">
         <f ca="1">NOW()</f>
-        <v>42462.368804861107</v>
+        <v>42464.504895138889</v>
       </c>
       <c r="D6" s="55"/>
       <c r="E6" s="55"/>
@@ -1493,8 +1480,8 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="12" thickBot="1"/>
-    <row r="8" spans="1:18" ht="23.25" customHeight="1" thickBot="1">
+    <row r="7" spans="1:16" ht="12" thickBot="1"/>
+    <row r="8" spans="1:16" ht="23.25" customHeight="1" thickBot="1">
       <c r="A8" s="38" t="s">
         <v>1</v>
       </c>
@@ -1506,7 +1493,7 @@
       </c>
       <c r="D8" s="58"/>
       <c r="E8" s="40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="40" t="s">
         <v>9</v>
@@ -1528,26 +1515,22 @@
         <v>13</v>
       </c>
       <c r="M8" s="57"/>
-      <c r="N8" s="57" t="s">
+      <c r="N8" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="57"/>
-      <c r="P8" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q8" s="43" t="s">
+      <c r="O8" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="R8" s="44" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" s="8" customFormat="1" ht="15.75">
+      <c r="P8" s="44" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" s="8" customFormat="1" ht="15.75">
       <c r="A9" s="16">
         <v>0</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="17">
         <v>35</v>
@@ -1556,7 +1539,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="37">
         <v>42434</v>
@@ -1571,39 +1554,33 @@
         <v>0</v>
       </c>
       <c r="J9" s="17">
-        <v>10</v>
+        <f>J12+J18+J24+J32</f>
+        <v>68</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L9" s="17">
         <v>7</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N9" s="17">
-        <f>J9-L9</f>
-        <v>3</v>
-      </c>
-      <c r="O9" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P9" s="18">
-        <f>SUM(P12,P18,P24,P32)/4</f>
-        <v>0.70624999999999993</v>
-      </c>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" s="8" customFormat="1" ht="15.75">
+        <v>17</v>
+      </c>
+      <c r="N9" s="18">
+        <f>SUM(N12,N18,N24,N32)/4</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="O9" s="19"/>
+      <c r="P9" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" s="8" customFormat="1" ht="15.75">
       <c r="A10" s="16">
         <v>0</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="17">
         <v>28</v>
@@ -1612,7 +1589,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="37">
         <v>42441</v>
@@ -1630,30 +1607,23 @@
         <v>8</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L10" s="17">
         <v>5</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N10" s="17">
-        <f>J10-L10</f>
-        <v>3</v>
-      </c>
-      <c r="O10" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P10" s="18">
+        <v>17</v>
+      </c>
+      <c r="N10" s="18">
         <v>0.7</v>
       </c>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" s="8" customFormat="1" ht="15.75">
+      <c r="O10" s="19"/>
+      <c r="P10" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="8" customFormat="1" ht="15.75">
       <c r="A11" s="16"/>
       <c r="B11" s="24"/>
       <c r="C11" s="17"/>
@@ -1667,18 +1637,16 @@
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="15"/>
-    </row>
-    <row r="12" spans="1:18" s="8" customFormat="1" ht="15">
+      <c r="N11" s="18"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="15"/>
+    </row>
+    <row r="12" spans="1:16" s="8" customFormat="1" ht="15">
       <c r="A12" s="16">
         <v>1</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="17">
         <v>7</v>
@@ -1687,7 +1655,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="37">
         <v>42434</v>
@@ -1702,38 +1670,31 @@
         <v>42440</v>
       </c>
       <c r="J12" s="17">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K12" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L12" s="17">
         <f>SUM(L13:L16)</f>
         <v>14</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N12" s="17">
-        <f t="shared" ref="N12:N22" si="0">J12-L12</f>
-        <v>-2</v>
-      </c>
-      <c r="O12" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P12" s="23">
-        <f>AVERAGE(P13:P16)</f>
-        <v>1</v>
-      </c>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="15"/>
-    </row>
-    <row r="13" spans="1:18" ht="15">
+        <v>17</v>
+      </c>
+      <c r="N12" s="18">
+        <f>AVERAGE(N13:N16)</f>
+        <v>1</v>
+      </c>
+      <c r="O12" s="19"/>
+      <c r="P12" s="15"/>
+    </row>
+    <row r="13" spans="1:16" ht="15">
       <c r="A13" s="16">
         <v>1.1000000000000001</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="17">
         <v>7</v>
@@ -1742,7 +1703,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13" s="37">
         <v>42434</v>
@@ -1760,35 +1721,28 @@
         <v>4</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L13" s="17">
         <v>8</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N13" s="17">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="O13" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P13" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="15">
+        <v>17</v>
+      </c>
+      <c r="N13" s="18">
+        <v>1</v>
+      </c>
+      <c r="O13" s="19"/>
+      <c r="P13" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15">
       <c r="A14" s="16">
         <v>1.2</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="17">
         <v>7</v>
@@ -1797,7 +1751,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" s="37">
         <v>42434</v>
@@ -1815,35 +1769,28 @@
         <v>2</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L14" s="17">
         <v>2</v>
       </c>
       <c r="M14" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N14" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P14" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="15">
+        <v>17</v>
+      </c>
+      <c r="N14" s="18">
+        <v>1</v>
+      </c>
+      <c r="O14" s="19"/>
+      <c r="P14" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15">
       <c r="A15" s="16">
         <v>1.3</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="17">
         <v>2</v>
@@ -1852,7 +1799,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" s="37">
         <v>42434</v>
@@ -1870,35 +1817,28 @@
         <v>2</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L15" s="17">
         <v>2</v>
       </c>
       <c r="M15" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N15" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P15" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="15">
+        <v>17</v>
+      </c>
+      <c r="N15" s="18">
+        <v>1</v>
+      </c>
+      <c r="O15" s="19"/>
+      <c r="P15" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15">
       <c r="A16" s="16">
         <v>1.4</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="17">
         <v>2</v>
@@ -1907,7 +1847,7 @@
         <v>8</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F16" s="37">
         <v>42434</v>
@@ -1925,30 +1865,23 @@
         <v>2</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L16" s="17">
         <v>2</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N16" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P16" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" s="34" customFormat="1" ht="15">
+        <v>17</v>
+      </c>
+      <c r="N16" s="18">
+        <v>1</v>
+      </c>
+      <c r="O16" s="19"/>
+      <c r="P16" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="34" customFormat="1" ht="15">
       <c r="A17" s="27"/>
       <c r="B17" s="28"/>
       <c r="C17" s="29"/>
@@ -1962,21 +1895,16 @@
       <c r="K17" s="29"/>
       <c r="L17" s="29"/>
       <c r="M17" s="29"/>
-      <c r="N17" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="29"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="33"/>
-    </row>
-    <row r="18" spans="1:18" s="8" customFormat="1" ht="15">
+      <c r="N17" s="31"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="33"/>
+    </row>
+    <row r="18" spans="1:16" s="8" customFormat="1" ht="15">
       <c r="A18" s="16">
         <v>2</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="17">
         <v>7</v>
@@ -1996,44 +1924,38 @@
       <c r="H18" s="37">
         <v>42447</v>
       </c>
-      <c r="I18" s="37" t="s">
-        <v>0</v>
+      <c r="I18" s="37">
+        <f>I22</f>
+        <v>42461</v>
       </c>
       <c r="J18" s="17">
         <v>12</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L18" s="17">
         <f>SUM(L19:L22)</f>
         <v>16</v>
       </c>
       <c r="M18" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N18" s="17">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="O18" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P18" s="18">
-        <f>AVERAGE(P19:P22)</f>
-        <v>0.92499999999999993</v>
-      </c>
-      <c r="Q18" s="19">
-        <v>1</v>
-      </c>
-      <c r="R18" s="15"/>
-    </row>
-    <row r="19" spans="1:18" ht="15">
+        <v>17</v>
+      </c>
+      <c r="N18" s="18">
+        <f>AVERAGE(N19:N22)</f>
+        <v>1</v>
+      </c>
+      <c r="O18" s="19">
+        <v>1</v>
+      </c>
+      <c r="P18" s="15"/>
+    </row>
+    <row r="19" spans="1:16" ht="15">
       <c r="A19" s="16">
         <v>2.1</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="17">
         <v>2</v>
@@ -2042,7 +1964,7 @@
         <v>8</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F19" s="37">
         <v>42441</v>
@@ -2060,35 +1982,28 @@
         <v>2</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L19" s="17">
         <v>4</v>
       </c>
       <c r="M19" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N19" s="17">
-        <f t="shared" si="0"/>
-        <v>-2</v>
-      </c>
-      <c r="O19" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P19" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="15">
+        <v>17</v>
+      </c>
+      <c r="N19" s="18">
+        <v>1</v>
+      </c>
+      <c r="O19" s="19"/>
+      <c r="P19" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15">
       <c r="A20" s="16">
         <v>2.2000000000000002</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="17">
         <v>2</v>
@@ -2115,37 +2030,30 @@
         <v>4</v>
       </c>
       <c r="K20" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L20" s="17">
         <v>6</v>
       </c>
       <c r="M20" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N20" s="17">
-        <f t="shared" si="0"/>
-        <v>-2</v>
-      </c>
-      <c r="O20" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P20" s="18">
-        <v>0.9</v>
-      </c>
-      <c r="Q20" s="19">
+        <v>17</v>
+      </c>
+      <c r="N20" s="18">
+        <v>1</v>
+      </c>
+      <c r="O20" s="19">
         <v>2.1</v>
       </c>
-      <c r="R20" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="15">
+      <c r="P20" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15">
       <c r="A21" s="16">
         <v>2.2999999999999998</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="17">
         <v>2</v>
@@ -2173,37 +2081,30 @@
         <v>4</v>
       </c>
       <c r="K21" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L21" s="17">
         <v>4</v>
       </c>
       <c r="M21" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N21" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O21" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P21" s="18">
-        <v>0.9</v>
-      </c>
-      <c r="Q21" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="R21" s="15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="15">
+        <v>17</v>
+      </c>
+      <c r="N21" s="18">
+        <v>1</v>
+      </c>
+      <c r="O21" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="P21" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15">
       <c r="A22" s="16">
         <v>2.4</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="17">
         <v>2</v>
@@ -2231,32 +2132,25 @@
         <v>2</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L22" s="17">
         <v>2</v>
       </c>
       <c r="M22" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N22" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O22" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P22" s="18">
-        <v>0.9</v>
-      </c>
-      <c r="Q22" s="19">
+        <v>17</v>
+      </c>
+      <c r="N22" s="18">
+        <v>1</v>
+      </c>
+      <c r="O22" s="19">
         <v>2.2000000000000002</v>
       </c>
-      <c r="R22" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" s="8" customFormat="1" ht="15">
+      <c r="P22" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" s="8" customFormat="1" ht="15">
       <c r="A23" s="16"/>
       <c r="B23" s="22"/>
       <c r="C23" s="17"/>
@@ -2270,18 +2164,16 @@
       <c r="K23" s="17"/>
       <c r="L23" s="17"/>
       <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="19"/>
-      <c r="R23" s="15"/>
-    </row>
-    <row r="24" spans="1:18" s="8" customFormat="1" ht="15">
+      <c r="N23" s="18"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="15"/>
+    </row>
+    <row r="24" spans="1:16" s="8" customFormat="1" ht="15">
       <c r="A24" s="16">
         <v>3</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="17">
         <v>14</v>
@@ -2301,45 +2193,38 @@
       <c r="H24" s="37">
         <v>42461</v>
       </c>
-      <c r="I24" s="37" t="s">
-        <v>0</v>
+      <c r="I24" s="37">
+        <f>I26</f>
+        <v>42462</v>
       </c>
       <c r="J24" s="17">
-        <f>SUM(J25:J30)+2</f>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K24" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L24" s="17">
         <f>SUM(L25:L30)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M24" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N24" s="17">
-        <f t="shared" ref="N24:N36" si="1">J24-L24</f>
-        <v>3</v>
-      </c>
-      <c r="O24" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P24" s="23">
-        <f>AVERAGE(P25:P30)</f>
-        <v>0.9</v>
-      </c>
-      <c r="Q24" s="19">
-        <v>2</v>
-      </c>
-      <c r="R24" s="15"/>
-    </row>
-    <row r="25" spans="1:18" ht="15">
+        <v>17</v>
+      </c>
+      <c r="N24" s="23">
+        <f>AVERAGE(N25:N30)</f>
+        <v>1</v>
+      </c>
+      <c r="O24" s="19">
+        <v>2</v>
+      </c>
+      <c r="P24" s="15"/>
+    </row>
+    <row r="25" spans="1:16" ht="15">
       <c r="A25" s="16">
         <v>3.1</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" s="17">
         <v>4</v>
@@ -2366,35 +2251,28 @@
         <v>4</v>
       </c>
       <c r="K25" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L25" s="17">
         <v>4</v>
       </c>
       <c r="M25" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N25" s="17">
-        <f>J25-L25</f>
-        <v>0</v>
-      </c>
-      <c r="O25" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P25" s="18">
-        <v>0.9</v>
-      </c>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="15">
+        <v>17</v>
+      </c>
+      <c r="N25" s="18">
+        <v>1</v>
+      </c>
+      <c r="O25" s="19"/>
+      <c r="P25" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="15">
       <c r="A26" s="16">
         <v>3.2</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="17">
         <v>4</v>
@@ -2423,37 +2301,30 @@
         <v>6</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L26" s="17">
         <v>6</v>
       </c>
       <c r="M26" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N26" s="17">
-        <f t="shared" ref="N26:N30" si="2">J26-L26</f>
-        <v>0</v>
-      </c>
-      <c r="O26" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P26" s="18">
-        <v>0.9</v>
-      </c>
-      <c r="Q26" s="19">
+        <v>17</v>
+      </c>
+      <c r="N26" s="18">
+        <v>1</v>
+      </c>
+      <c r="O26" s="19">
         <v>3.1</v>
       </c>
-      <c r="R26" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" ht="15">
+      <c r="P26" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="15">
       <c r="A27" s="16">
         <v>3.3</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C27" s="17">
         <v>1</v>
@@ -2481,37 +2352,30 @@
         <v>2</v>
       </c>
       <c r="K27" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L27" s="17">
         <v>2</v>
       </c>
       <c r="M27" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N27" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O27" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P27" s="18">
-        <v>0.9</v>
-      </c>
-      <c r="Q27" s="19">
+        <v>17</v>
+      </c>
+      <c r="N27" s="18">
+        <v>1</v>
+      </c>
+      <c r="O27" s="19">
         <v>3.2</v>
       </c>
-      <c r="R27" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="15">
+      <c r="P27" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="15">
       <c r="A28" s="16">
         <v>3.4</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" s="17">
         <v>2</v>
@@ -2539,37 +2403,30 @@
         <v>6</v>
       </c>
       <c r="K28" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L28" s="17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M28" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N28" s="17">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O28" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P28" s="18">
-        <v>0.8</v>
-      </c>
-      <c r="Q28" s="19">
+        <v>17</v>
+      </c>
+      <c r="N28" s="18">
+        <v>1</v>
+      </c>
+      <c r="O28" s="19">
         <v>3.2</v>
       </c>
-      <c r="R28" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="15">
+      <c r="P28" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="15">
       <c r="A29" s="16">
         <v>3.5</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="17">
         <v>1</v>
@@ -2597,37 +2454,30 @@
         <v>2</v>
       </c>
       <c r="K29" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L29" s="17">
         <v>2</v>
       </c>
       <c r="M29" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N29" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O29" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P29" s="18">
-        <v>0.9</v>
-      </c>
-      <c r="Q29" s="19">
+        <v>17</v>
+      </c>
+      <c r="N29" s="18">
+        <v>1</v>
+      </c>
+      <c r="O29" s="19">
         <v>3.4</v>
       </c>
-      <c r="R29" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="15">
+      <c r="P29" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="15">
       <c r="A30" s="16">
         <v>3.6</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C30" s="17">
         <v>2</v>
@@ -2636,7 +2486,7 @@
         <v>8</v>
       </c>
       <c r="E30" s="36" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F30" s="37">
         <v>42455</v>
@@ -2654,30 +2504,23 @@
         <v>2</v>
       </c>
       <c r="K30" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L30" s="17">
         <v>2</v>
       </c>
       <c r="M30" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N30" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O30" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P30" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" s="34" customFormat="1" ht="15">
+        <v>17</v>
+      </c>
+      <c r="N30" s="18">
+        <v>1</v>
+      </c>
+      <c r="O30" s="19"/>
+      <c r="P30" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" s="34" customFormat="1" ht="15">
       <c r="A31" s="27"/>
       <c r="B31" s="28"/>
       <c r="C31" s="29"/>
@@ -2691,18 +2534,16 @@
       <c r="K31" s="29"/>
       <c r="L31" s="29"/>
       <c r="M31" s="29"/>
-      <c r="N31" s="17"/>
-      <c r="O31" s="29"/>
-      <c r="P31" s="31"/>
-      <c r="Q31" s="32"/>
-      <c r="R31" s="33"/>
-    </row>
-    <row r="32" spans="1:18" s="8" customFormat="1" ht="15">
+      <c r="N31" s="31"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="33"/>
+    </row>
+    <row r="32" spans="1:16" s="8" customFormat="1" ht="15">
       <c r="A32" s="16">
         <v>2</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C32" s="17">
         <v>7</v>
@@ -2711,16 +2552,16 @@
         <v>8</v>
       </c>
       <c r="E32" s="36" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F32" s="37">
         <v>42462</v>
       </c>
-      <c r="G32" s="37" t="s">
-        <v>0</v>
+      <c r="G32" s="37">
+        <v>42463</v>
       </c>
       <c r="H32" s="37">
-        <v>42468</v>
+        <v>42469</v>
       </c>
       <c r="I32" s="37" t="s">
         <v>0</v>
@@ -2729,34 +2570,28 @@
         <v>24</v>
       </c>
       <c r="K32" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L32" s="17">
-        <v>0</v>
+        <f>SUM(L33:L41)</f>
+        <v>7</v>
       </c>
       <c r="M32" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N32" s="17">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="O32" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P32" s="18">
-        <f>AVERAGE(P33:P36)</f>
-        <v>0</v>
-      </c>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="15"/>
-    </row>
-    <row r="33" spans="1:18" ht="15">
+        <v>17</v>
+      </c>
+      <c r="N32" s="18">
+        <f>AVERAGE(N35:N41)</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="O32" s="19"/>
+      <c r="P32" s="15"/>
+    </row>
+    <row r="33" spans="1:16" ht="15">
       <c r="A33" s="16">
         <v>2.1</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C33" s="17">
         <v>1</v>
@@ -2765,108 +2600,94 @@
         <v>8</v>
       </c>
       <c r="E33" s="36" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="F33" s="37">
         <v>42462</v>
       </c>
-      <c r="G33" s="37" t="s">
-        <v>0</v>
+      <c r="G33" s="37">
+        <v>42463</v>
       </c>
       <c r="H33" s="37">
-        <v>42468</v>
-      </c>
-      <c r="I33" s="37" t="s">
-        <v>0</v>
+        <v>42463</v>
+      </c>
+      <c r="I33" s="37">
+        <v>42464</v>
       </c>
       <c r="J33" s="17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K33" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L33" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N33" s="17">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="O33" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P33" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="19"/>
-      <c r="R33" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" ht="15">
+        <v>17</v>
+      </c>
+      <c r="N33" s="18">
+        <v>1</v>
+      </c>
+      <c r="O33" s="19"/>
+      <c r="P33" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="15">
       <c r="A34" s="16">
-        <v>2.2999999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="C34" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="36" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="F34" s="37">
         <v>42462</v>
       </c>
-      <c r="G34" s="37" t="s">
-        <v>0</v>
+      <c r="G34" s="37">
+        <v>42463</v>
       </c>
       <c r="H34" s="37">
-        <v>42468</v>
-      </c>
-      <c r="I34" s="37" t="s">
-        <v>0</v>
+        <v>42464</v>
+      </c>
+      <c r="I34" s="37">
+        <v>42464</v>
       </c>
       <c r="J34" s="17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K34" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L34" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M34" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N34" s="17">
-        <f>J34-L34</f>
-        <v>4</v>
-      </c>
-      <c r="O34" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P34" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="35"/>
-      <c r="R34" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" ht="15">
+        <v>17</v>
+      </c>
+      <c r="N34" s="18">
+        <v>1</v>
+      </c>
+      <c r="O34" s="19"/>
+      <c r="P34" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="15">
       <c r="A35" s="16">
-        <v>2.2000000000000002</v>
+        <v>2.1</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C35" s="17">
         <v>2</v>
@@ -2875,53 +2696,46 @@
         <v>8</v>
       </c>
       <c r="E35" s="36" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="F35" s="37">
         <v>42462</v>
       </c>
-      <c r="G35" s="37" t="s">
-        <v>0</v>
+      <c r="G35" s="37">
+        <v>42463</v>
       </c>
       <c r="H35" s="37">
-        <v>42468</v>
-      </c>
-      <c r="I35" s="37" t="s">
-        <v>0</v>
+        <v>42464</v>
+      </c>
+      <c r="I35" s="37">
+        <v>42469</v>
       </c>
       <c r="J35" s="17">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K35" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L35" s="17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M35" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N35" s="17">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="O35" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P35" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="19"/>
-      <c r="R35" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" ht="15">
+        <v>17</v>
+      </c>
+      <c r="N35" s="18">
+        <v>1</v>
+      </c>
+      <c r="O35" s="19"/>
+      <c r="P35" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="15">
       <c r="A36" s="16">
         <v>2.4</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C36" s="17">
         <v>2</v>
@@ -2930,73 +2744,304 @@
         <v>8</v>
       </c>
       <c r="E36" s="36" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="F36" s="37">
+        <v>42463</v>
+      </c>
+      <c r="G36" s="37">
+        <v>42463</v>
+      </c>
+      <c r="H36" s="37">
+        <v>42465</v>
+      </c>
+      <c r="I36" s="37">
+        <v>42469</v>
+      </c>
+      <c r="J36" s="17">
+        <v>2</v>
+      </c>
+      <c r="K36" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="17">
+        <v>2</v>
+      </c>
+      <c r="M36" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="N36" s="18">
+        <v>1</v>
+      </c>
+      <c r="O36" s="19"/>
+      <c r="P36" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="15">
+      <c r="A37" s="16">
+        <v>2.1</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="17">
+        <v>1</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="37">
+        <v>42464</v>
+      </c>
+      <c r="G37" s="37">
+        <f>I33</f>
+        <v>42464</v>
+      </c>
+      <c r="H37" s="37">
+        <v>42465</v>
+      </c>
+      <c r="I37" s="37">
+        <v>42469</v>
+      </c>
+      <c r="J37" s="17">
+        <v>1</v>
+      </c>
+      <c r="K37" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="L37" s="17">
+        <v>1</v>
+      </c>
+      <c r="M37" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="N37" s="18">
+        <v>1</v>
+      </c>
+      <c r="O37" s="19"/>
+      <c r="P37" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="15">
+      <c r="A38" s="16">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="17">
+        <v>2</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" s="37">
         <v>42462</v>
       </c>
-      <c r="G36" s="37" t="s">
+      <c r="G38" s="37">
+        <v>42469</v>
+      </c>
+      <c r="H38" s="37">
+        <v>42468</v>
+      </c>
+      <c r="I38" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="H36" s="37">
+      <c r="J38" s="17">
+        <v>4</v>
+      </c>
+      <c r="K38" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="L38" s="17">
+        <v>0</v>
+      </c>
+      <c r="M38" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="N38" s="18">
+        <v>0</v>
+      </c>
+      <c r="O38" s="35"/>
+      <c r="P38" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="15">
+      <c r="A39" s="16">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="17">
+        <v>2</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" s="37">
+        <v>42462</v>
+      </c>
+      <c r="G39" s="37">
+        <v>42469</v>
+      </c>
+      <c r="H39" s="37">
         <v>42468</v>
       </c>
-      <c r="I36" s="37" t="s">
+      <c r="I39" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="J36" s="17">
+      <c r="J39" s="17">
         <v>4</v>
       </c>
-      <c r="K36" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="L36" s="17">
+      <c r="K39" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="L39" s="17">
         <v>0</v>
       </c>
-      <c r="M36" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="N36" s="17">
-        <f t="shared" si="1"/>
+      <c r="M39" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="N39" s="18">
+        <v>0</v>
+      </c>
+      <c r="O39" s="35"/>
+      <c r="P39" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="15">
+      <c r="A40" s="16">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="17">
+        <v>2</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F40" s="37">
+        <v>42462</v>
+      </c>
+      <c r="G40" s="37">
+        <v>42469</v>
+      </c>
+      <c r="H40" s="37">
+        <v>42468</v>
+      </c>
+      <c r="I40" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="J40" s="17">
         <v>4</v>
       </c>
-      <c r="O36" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="P36" s="18">
+      <c r="K40" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="L40" s="17">
         <v>0</v>
       </c>
-      <c r="Q36" s="19"/>
-      <c r="R36" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" ht="15">
-      <c r="A37" s="16"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="17"/>
-      <c r="O37" s="17"/>
-      <c r="P37" s="18"/>
-      <c r="Q37" s="19"/>
-      <c r="R37" s="15"/>
+      <c r="M40" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="N40" s="18">
+        <v>0</v>
+      </c>
+      <c r="O40" s="19"/>
+      <c r="P40" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="15">
+      <c r="A41" s="16">
+        <v>2.4</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="17">
+        <v>2</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F41" s="37">
+        <v>42469</v>
+      </c>
+      <c r="G41" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="37">
+        <v>42469</v>
+      </c>
+      <c r="I41" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="J41" s="17">
+        <v>4</v>
+      </c>
+      <c r="K41" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="L41" s="17">
+        <v>0</v>
+      </c>
+      <c r="M41" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="N41" s="18">
+        <v>0</v>
+      </c>
+      <c r="O41" s="19"/>
+      <c r="P41" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="15">
+      <c r="A42" s="16"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C6:F6"/>
-    <mergeCell ref="N8:O8"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="C8:D8"/>

</xml_diff>